<commit_message>
finished every function except generate summary report
</commit_message>
<xml_diff>
--- a/BluePear/php/evaluations/Louel.xlsx
+++ b/BluePear/php/evaluations/Louel.xlsx
@@ -89,14 +89,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Rating: 4</t>
+          <t>Rating: 1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Comment: ASDF11</t>
+          <t>Comment: asdf</t>
         </is>
       </c>
     </row>
@@ -110,14 +110,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Rating: 4</t>
+          <t>Rating: 3</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Comment: ASDF12</t>
+          <t>Comment: asdf</t>
         </is>
       </c>
     </row>
@@ -143,14 +143,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rating: 1</t>
+          <t>Rating: 5</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Comment: ASDF21</t>
+          <t>Comment: qwer</t>
         </is>
       </c>
     </row>
@@ -164,14 +164,14 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Rating: 1</t>
+          <t>Rating: 3</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Comment: ASDF22</t>
+          <t>Comment: qwer</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adjusted a few prompts
</commit_message>
<xml_diff>
--- a/BluePear/php/evaluations/Louel.xlsx
+++ b/BluePear/php/evaluations/Louel.xlsx
@@ -96,7 +96,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Comment: asdf</t>
+          <t>Comment: Louel</t>
         </is>
       </c>
     </row>
@@ -110,14 +110,14 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Rating: 3</t>
+          <t>Rating: 2</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Comment: asdf</t>
+          <t>Comment: Yes</t>
         </is>
       </c>
     </row>
@@ -143,14 +143,14 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Rating: 5</t>
+          <t>Rating: 1</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Comment: qwer</t>
+          <t>Comment: Haha</t>
         </is>
       </c>
     </row>
@@ -171,7 +171,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Comment: qwer</t>
+          <t>Comment: Lolz</t>
         </is>
       </c>
     </row>

</xml_diff>